<commit_message>
Reformated file contents for submission
</commit_message>
<xml_diff>
--- a/primary_analysis/summary_table_percent_change.xlsx
+++ b/primary_analysis/summary_table_percent_change.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ujjwal\viagogo_case_study\primary_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FD58309-90CF-497C-ACC4-F539D982EC32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B761AC6-DE07-46DC-9165-B3055035F946}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{19449B45-6BB2-45A3-AD5C-4A6F4E119AE6}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="18">
   <si>
     <t>Channel</t>
   </si>
@@ -72,14 +72,30 @@
   </si>
   <si>
     <t>Affiliate</t>
+  </si>
+  <si>
+    <t>Conversion Rate</t>
+  </si>
+  <si>
+    <t>Bounce Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bounce Rate </t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>Variant</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="171" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -90,7 +106,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -115,8 +131,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -422,11 +456,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -470,75 +533,107 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,10 +642,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCC0000"/>
+      <color rgb="FFFFFFFF"/>
       <color rgb="FF66FF33"/>
       <color rgb="FFF13D3D"/>
-      <color rgb="FFFFFFFF"/>
-      <color rgb="FFCC0000"/>
     </mruColors>
   </colors>
   <extLst>
@@ -861,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52D66136-7517-4B18-B816-33F9CF7A6ACF}">
-  <dimension ref="B2:K12"/>
+  <dimension ref="B2:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,9 +968,9 @@
     <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="29.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="14" style="1" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1"/>
+    <col min="5" max="6" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="8" max="8" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
     <col min="10" max="10" width="12.140625" style="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="1"/>
@@ -884,21 +979,21 @@
     <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="14"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="26" t="s">
+      <c r="C3" s="25"/>
+      <c r="D3" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="16"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="34"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="32"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="27" t="s">
+      <c r="B4" s="26"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="22" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -916,15 +1011,15 @@
       <c r="I4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="17" t="s">
+      <c r="J4" s="15" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="23" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="9">
@@ -942,16 +1037,16 @@
       <c r="H5" s="6">
         <v>-4.9599999999999998E-2</v>
       </c>
-      <c r="I5" s="37">
+      <c r="I5" s="31">
         <v>3.8E-3</v>
       </c>
-      <c r="J5" s="19">
+      <c r="J5" s="16">
         <v>-1.0500000000000001E-2</v>
       </c>
       <c r="K5" s="8"/>
     </row>
     <row r="6" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="18"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
@@ -973,13 +1068,13 @@
       <c r="I6" s="7">
         <v>1.9599999999999999E-2</v>
       </c>
-      <c r="J6" s="20">
+      <c r="J6" s="17">
         <v>2.3400000000000001E-2</v>
       </c>
       <c r="K6" s="8"/>
     </row>
     <row r="7" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="36" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1000,15 +1095,15 @@
       <c r="H7" s="6">
         <v>-4.19E-2</v>
       </c>
-      <c r="I7" s="33">
+      <c r="I7" s="27">
         <v>3.3999999999999998E-3</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7" s="16">
         <v>2.7799999999999998E-2</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="18"/>
+      <c r="B8" s="36"/>
       <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
@@ -1027,15 +1122,15 @@
       <c r="H8" s="7">
         <v>4.6300000000000001E-2</v>
       </c>
-      <c r="I8" s="34">
+      <c r="I8" s="28">
         <v>-2.2599999999999999E-2</v>
       </c>
-      <c r="J8" s="20">
+      <c r="J8" s="17">
         <v>2.0400000000000001E-2</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="36" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -1050,7 +1145,7 @@
       <c r="F9" s="6">
         <v>-5.2200000000000003E-2</v>
       </c>
-      <c r="G9" s="35">
+      <c r="G9" s="29">
         <v>-0.10199999999999999</v>
       </c>
       <c r="H9" s="6">
@@ -1059,34 +1154,34 @@
       <c r="I9" s="6">
         <v>-8.0000000000000002E-3</v>
       </c>
-      <c r="J9" s="19">
+      <c r="J9" s="16">
         <v>-4.7699999999999999E-2</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="21"/>
-      <c r="C10" s="22" t="s">
+      <c r="B10" s="37"/>
+      <c r="C10" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="19">
         <v>4.3799999999999999E-2</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="20">
         <v>6.4699999999999994E-2</v>
       </c>
-      <c r="F10" s="24">
+      <c r="F10" s="20">
         <v>4.7500000000000001E-2</v>
       </c>
-      <c r="G10" s="36">
+      <c r="G10" s="30">
         <v>2.5899999999999999E-2</v>
       </c>
-      <c r="H10" s="24">
+      <c r="H10" s="20">
         <v>1.2699999999999999E-2</v>
       </c>
-      <c r="I10" s="24">
+      <c r="I10" s="20">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="J10" s="25">
+      <c r="J10" s="21">
         <v>2.92E-2</v>
       </c>
     </row>
@@ -1099,12 +1194,444 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
+    <row r="15" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="39"/>
+      <c r="D16" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="34"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="40"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="L17" s="50"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="42">
+        <v>5.5613329000000003E-2</v>
+      </c>
+      <c r="E18" s="42">
+        <v>5.5017619449156098E-2</v>
+      </c>
+      <c r="F18" s="42">
+        <v>5.9182272651208997E-2</v>
+      </c>
+      <c r="G18" s="42">
+        <v>5.7279105065758999E-2</v>
+      </c>
+      <c r="H18" s="42">
+        <v>5.3535126417638898E-2</v>
+      </c>
+      <c r="I18" s="42">
+        <v>6.2975086707970293E-2</v>
+      </c>
+      <c r="J18" s="47">
+        <v>5.5510236855386801E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="36"/>
+      <c r="C19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="43">
+        <v>0.396011432</v>
+      </c>
+      <c r="E19" s="43">
+        <v>0.39213408973474401</v>
+      </c>
+      <c r="F19" s="43">
+        <v>0.389426893872799</v>
+      </c>
+      <c r="G19" s="43">
+        <v>0.40817553866072998</v>
+      </c>
+      <c r="H19" s="43">
+        <v>0.39535728272154003</v>
+      </c>
+      <c r="I19" s="43">
+        <v>0.40044385376876901</v>
+      </c>
+      <c r="J19" s="48">
+        <v>0.400110838721771</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="42">
+        <v>5.2955672877066998E-2</v>
+      </c>
+      <c r="E20" s="42">
+        <v>5.3703159533305497E-2</v>
+      </c>
+      <c r="F20" s="42">
+        <v>5.3574919897910502E-2</v>
+      </c>
+      <c r="G20" s="53">
+        <v>5.2227428271899502E-2</v>
+      </c>
+      <c r="H20" s="42">
+        <v>5.2268327086171802E-2</v>
+      </c>
+      <c r="I20" s="42">
+        <v>5.5182127192582399E-2</v>
+      </c>
+      <c r="J20" s="47">
+        <v>5.27763162632418E-2</v>
+      </c>
+      <c r="L20" s="50"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="36"/>
+      <c r="C21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="43">
+        <v>0.39848390717393201</v>
+      </c>
+      <c r="E21" s="43">
+        <v>0.393445340509257</v>
+      </c>
+      <c r="F21" s="43">
+        <v>0.40315370912290399</v>
+      </c>
+      <c r="G21" s="54">
+        <v>0.415155254946382</v>
+      </c>
+      <c r="H21" s="43">
+        <v>0.39252982315726997</v>
+      </c>
+      <c r="I21" s="43">
+        <v>0.40921659819325601</v>
+      </c>
+      <c r="J21" s="48">
+        <v>0.401909819417193</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="42">
+        <v>5.9565371057441301E-2</v>
+      </c>
+      <c r="E22" s="42">
+        <v>5.7325883437755E-2</v>
+      </c>
+      <c r="F22" s="55">
+        <v>6.7755756915942697E-2</v>
+      </c>
+      <c r="G22" s="42">
+        <v>6.4983272729031996E-2</v>
+      </c>
+      <c r="H22" s="42">
+        <v>5.59056313366652E-2</v>
+      </c>
+      <c r="I22" s="51">
+        <v>7.6108666839487402E-2</v>
+      </c>
+      <c r="J22" s="44">
+        <v>5.9858793971026399E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="37"/>
+      <c r="C23" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="45">
+        <v>0.39266798341363701</v>
+      </c>
+      <c r="E23" s="45">
+        <v>0.389806972440082</v>
+      </c>
+      <c r="F23" s="56">
+        <v>0.37053366553539002</v>
+      </c>
+      <c r="G23" s="45">
+        <v>0.39797293485350099</v>
+      </c>
+      <c r="H23" s="45">
+        <v>0.40209093047277999</v>
+      </c>
+      <c r="I23" s="52">
+        <v>0.389723840943422</v>
+      </c>
+      <c r="J23" s="46">
+        <v>0.39718581416926302</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="39"/>
+      <c r="D25" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="34"/>
+      <c r="L25" s="50"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="40"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J26" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="L26" s="50"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="42">
+        <v>5.3105799000000002E-2</v>
+      </c>
+      <c r="E27" s="42">
+        <v>5.16422630614745E-2</v>
+      </c>
+      <c r="F27" s="42">
+        <v>5.5593563530896797E-2</v>
+      </c>
+      <c r="G27" s="42">
+        <v>5.4681934878392999E-2</v>
+      </c>
+      <c r="H27" s="42">
+        <v>5.0882163172531497E-2</v>
+      </c>
+      <c r="I27" s="51">
+        <v>6.3213952037958196E-2</v>
+      </c>
+      <c r="J27" s="47">
+        <v>5.4928068907498101E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="36"/>
+      <c r="C28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="43">
+        <v>0.411870393</v>
+      </c>
+      <c r="E28" s="43">
+        <v>0.41322415580766098</v>
+      </c>
+      <c r="F28" s="43">
+        <v>0.40518659801287799</v>
+      </c>
+      <c r="G28" s="43">
+        <v>0.42286575386876901</v>
+      </c>
+      <c r="H28" s="43">
+        <v>0.40964239216703402</v>
+      </c>
+      <c r="I28" s="59">
+        <v>0.40827435545445101</v>
+      </c>
+      <c r="J28" s="48">
+        <v>0.40948491164196599</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="42">
+        <v>5.1371543318540297E-2</v>
+      </c>
+      <c r="E29" s="42">
+        <v>5.0771766864411101E-2</v>
+      </c>
+      <c r="F29" s="42">
+        <v>5.0362132592926399E-2</v>
+      </c>
+      <c r="G29" s="42">
+        <v>5.2589640015920598E-2</v>
+      </c>
+      <c r="H29" s="57">
+        <v>5.0076022167286301E-2</v>
+      </c>
+      <c r="I29" s="51">
+        <v>5.5369944604090601E-2</v>
+      </c>
+      <c r="J29" s="47">
+        <v>5.4241144666439499E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="36"/>
+      <c r="C30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="43">
+        <v>0.41307317861324899</v>
+      </c>
+      <c r="E30" s="43">
+        <v>0.41141886607869399</v>
+      </c>
+      <c r="F30" s="43">
+        <v>0.41710431872764597</v>
+      </c>
+      <c r="G30" s="43">
+        <v>0.43293120112108702</v>
+      </c>
+      <c r="H30" s="58">
+        <v>0.410706839856051</v>
+      </c>
+      <c r="I30" s="59">
+        <v>0.39996818067793399</v>
+      </c>
+      <c r="J30" s="48">
+        <v>0.410119763559401</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B31" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="42">
+        <v>5.5783159283179701E-2</v>
+      </c>
+      <c r="E31" s="42">
+        <v>5.32707432336159E-2</v>
+      </c>
+      <c r="F31" s="51">
+        <v>6.4219134596889396E-2</v>
+      </c>
+      <c r="G31" s="42">
+        <v>5.8362839032482697E-2</v>
+      </c>
+      <c r="H31" s="42">
+        <v>5.2587073381092503E-2</v>
+      </c>
+      <c r="I31" s="51">
+        <v>7.5502348107108305E-2</v>
+      </c>
+      <c r="J31" s="47">
+        <v>5.7003936995804E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="37"/>
+      <c r="C32" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="45">
+        <v>0.40988029872370602</v>
+      </c>
+      <c r="E32" s="45">
+        <v>0.41503194369083801</v>
+      </c>
+      <c r="F32" s="52">
+        <v>0.38813189817967297</v>
+      </c>
+      <c r="G32" s="45">
+        <v>0.40826548398388701</v>
+      </c>
+      <c r="H32" s="45">
+        <v>0.40718598319548699</v>
+      </c>
+      <c r="I32" s="52">
+        <v>0.42170025223051999</v>
+      </c>
+      <c r="J32" s="49">
+        <v>0.40878307469212699</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="14">
+    <mergeCell ref="D25:J25"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="B25:C26"/>
     <mergeCell ref="D3:J3"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B9:B10"/>
+    <mergeCell ref="D16:J16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>